<commit_message>
Add README graph to xlsx file
Also format the output from the perf program so that it's very easy to block select and copy from the console into Excel to update the data.
</commit_message>
<xml_diff>
--- a/graph.xlsx
+++ b/graph.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21310"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neuecc\Documents\neuecc\MessagePack\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\MessagePack-CSharp\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C89E4D-52EA-4D61-B931-0C492B106DB4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="53925" windowHeight="28320"/>
+    <workbookView xWindow="48480" yWindow="-3600" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="README graph" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,64 +25,132 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={675115CE-AC10-4A12-9B1A-05563BDC58F9}</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{675115CE-AC10-4A12-9B1A-05563BDC58F9}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Regenerate/refresh this data using the sandbox\PerfNetFramework program.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
   <si>
     <t>Small Object(int, string, stringm enum)</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>MessagePack C#</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>MsgPack-Cli</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>protobuf-net</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>ZeroFormatter</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Serialize</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Deserialize</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>FileSize</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Large Array(Small Object[1000])</t>
-    <phoneticPr fontId="1"/>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>protobuf-net</t>
+  </si>
+  <si>
+    <t>ZeroFormatter</t>
+  </si>
+  <si>
+    <t>MsgPack-Cli</t>
+  </si>
+  <si>
+    <t>FileSize::</t>
+  </si>
+  <si>
+    <t>Deserialize::</t>
+  </si>
+  <si>
+    <t>Serialize::</t>
+  </si>
+  <si>
+    <t>MessagePack for C#</t>
+  </si>
+  <si>
+    <t>MessagePack for C# (LZ4)</t>
+  </si>
+  <si>
+    <t>Json.NET</t>
+  </si>
+  <si>
+    <t>Json.NET(+GZip)</t>
+  </si>
+  <si>
+    <t>c405c58cbf (origin/master)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0\ &quot;bytes&quot;"/>
+    <numFmt numFmtId="165" formatCode="#,#00\ &quot;ms&quot;"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -100,18 +170,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{EEED627A-A0C2-4276-9DBE-5120BEC3B1C1}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -129,7 +207,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="ja-JP"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -148,6 +226,605 @@
           <a:p>
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Person[100], 10K iterations</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Serialize</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'README graph'!$A$3:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>MessagePack for C#</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MessagePack for C# (LZ4)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MsgPack-Cli</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>protobuf-net</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ZeroFormatter</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Json.NET</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Json.NET(+GZip)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'README graph'!$B$3:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>#,#00\ "ms"</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>137.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>160.72999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>335.23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>449.62</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>141.72999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1543.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1680.56</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F24E-46C8-97F4-2E2259F68447}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Deserialize</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'README graph'!$B$12:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>#,#00\ "ms"</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>177.33</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>182.04</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1106.8699999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>627.23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>139.91</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1876.02</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2237.38</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F24E-46C8-97F4-2E2259F68447}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="644809744"/>
+        <c:axId val="644811056"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'README graph'!$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FileSize::</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'README graph'!$B$21:$B$27</c:f>
+              <c:numCache>
+                <c:formatCode>0\ "bytes"</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1803</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>562</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2347</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2248</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6096</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>458</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F24E-46C8-97F4-2E2259F68447}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="448822072"/>
+        <c:axId val="448823384"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="644809744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="644811056"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="644811056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,#00\ &quot;ms&quot;" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="644809744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="448823384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="0\ &quot;bytes&quot;" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="448822072"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="448822072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="448823384"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="ja-JP" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -188,7 +865,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr lang="ja-JP" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -200,7 +877,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ja-JP"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -273,7 +950,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr lang="ja-JP" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -285,7 +962,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="ja-JP"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -403,7 +1080,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr lang="ja-JP" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -415,7 +1092,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="ja-JP"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -533,7 +1210,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr lang="ja-JP" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -545,7 +1222,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="ja-JP"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -663,7 +1340,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr lang="ja-JP" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -675,7 +1352,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="ja-JP"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -783,7 +1460,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="ja-JP" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -795,7 +1472,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ja-JP"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="684191056"/>
@@ -844,7 +1521,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr lang="ja-JP" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -856,7 +1533,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ja-JP"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -886,7 +1563,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="ja-JP"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -897,10 +1574,10 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="ja-JP"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -918,7 +1595,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr lang="ja-JP" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -957,7 +1634,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr lang="ja-JP" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -969,7 +1646,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ja-JP"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1019,7 +1696,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr lang="ja-JP" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -1031,7 +1708,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="ja-JP"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -1136,7 +1813,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr lang="ja-JP" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -1148,7 +1825,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="ja-JP"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -1253,7 +1930,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr lang="ja-JP" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -1265,7 +1942,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="ja-JP"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -1370,7 +2047,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr lang="ja-JP" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -1382,7 +2059,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="ja-JP"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -1490,7 +2167,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="ja-JP" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1502,7 +2179,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ja-JP"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="763540168"/>
@@ -1550,7 +2227,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr lang="ja-JP" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1562,7 +2239,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ja-JP"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1592,7 +2269,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="ja-JP"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1683,8 +2360,48 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1888,23 +2605,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -2009,8 +2725,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2142,20 +2858,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2693,7 +3408,555 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>100013</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8CD590D-F1DD-41DC-8CF1-24EF13F18E45}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2770,8 +4033,14 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Andrew Arnott" id="{741C964C-831C-49B3-8C72-00961BB146EB}" userId="S::andarno@microsoft.com::fef1612b-3282-4fb1-9982-6bb0b7d12ab8" providerId="AD"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3065,22 +4334,252 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B1" dT="2019-01-27T03:35:00.29" personId="{741C964C-831C-49B3-8C72-00961BB146EB}" id="{675115CE-AC10-4A12-9B1A-05563BDC58F9}">
+    <text>Regenerate/refresh this data using the sandbox\PerfNetFramework program.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C478671A-2BFF-4005-AC60-F5FFFBF24A55}">
+  <dimension ref="A1:B27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="19.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.46484375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.06640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="4">
+        <v>137.69999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="4">
+        <v>160.72999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="4">
+        <v>335.23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4">
+        <v>449.62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4">
+        <v>141.72999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1543.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1680.56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="4">
+        <v>177.33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="4">
+        <v>182.04</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="4">
+        <v>1106.8699999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="4">
+        <v>627.23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="4">
+        <v>139.91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="4">
+        <v>1876.02</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="4">
+        <v>2237.38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="3"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1803</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="2">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="2">
+        <v>2347</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="2">
+        <v>2248</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="2">
+        <v>5004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="2">
+        <v>6096</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="2">
+        <v>458</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="H8:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="8" max="8" width="10.46484375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="8" spans="8:12" x14ac:dyDescent="0.4">
+    <row r="8" spans="8:12">
       <c r="I8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="8:12" x14ac:dyDescent="0.4">
+    <row r="9" spans="8:12">
       <c r="I9" t="s">
         <v>1</v>
       </c>
@@ -3094,7 +4593,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="8:12" x14ac:dyDescent="0.4">
+    <row r="10" spans="8:12">
       <c r="H10" t="s">
         <v>5</v>
       </c>
@@ -3111,7 +4610,7 @@
         <v>1.5387999999999999</v>
       </c>
     </row>
-    <row r="11" spans="8:12" x14ac:dyDescent="0.4">
+    <row r="11" spans="8:12">
       <c r="H11" t="s">
         <v>6</v>
       </c>
@@ -3128,7 +4627,7 @@
         <v>1.3212999999999999</v>
       </c>
     </row>
-    <row r="12" spans="8:12" x14ac:dyDescent="0.4">
+    <row r="12" spans="8:12">
       <c r="H12" t="s">
         <v>7</v>
       </c>
@@ -3145,12 +4644,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="8:12" x14ac:dyDescent="0.4">
+    <row r="15" spans="8:12">
       <c r="I15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="8:12" x14ac:dyDescent="0.4">
+    <row r="16" spans="8:12">
       <c r="I16" t="s">
         <v>1</v>
       </c>
@@ -3164,7 +4663,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="8:12" x14ac:dyDescent="0.4">
+    <row r="17" spans="8:12">
       <c r="H17" t="s">
         <v>5</v>
       </c>
@@ -3181,7 +4680,7 @@
         <v>118.71899999999999</v>
       </c>
     </row>
-    <row r="18" spans="8:12" x14ac:dyDescent="0.4">
+    <row r="18" spans="8:12">
       <c r="H18" t="s">
         <v>6</v>
       </c>
@@ -3198,7 +4697,7 @@
         <v>165.98670000000001</v>
       </c>
     </row>
-    <row r="19" spans="8:12" x14ac:dyDescent="0.4">
+    <row r="19" spans="8:12">
       <c r="H19" t="s">
         <v>7</v>
       </c>
@@ -3216,8 +4715,9 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1"/>
+  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>